<commit_message>
Corrected the coordinates for Tiergartenstraße 3 (69120 Heidelberg), which were previously outside the city area due to a data error. Used Google Maps to approximate accurate location: 49.4195, 8.6593. Due to recent access restrictions on the Eurodata website, it was not possible to verify or update the original source data as of June 2025.
</commit_message>
<xml_diff>
--- a/datas/new_ladesaulen_hd.xlsx
+++ b/datas/new_ladesaulen_hd.xlsx
@@ -455,10 +455,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -543,7 +542,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,24 +551,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -766,91 +753,104 @@
   </sheetPr>
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W:W"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="13.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="33.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="26.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="33.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="27.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -864,7 +864,7 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>69066</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -909,7 +909,7 @@
       <c r="V2" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W2" s="2" t="n">
+      <c r="W2" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -923,7 +923,7 @@
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -968,7 +968,7 @@
       <c r="V3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W3" s="2" t="n">
+      <c r="W3" s="1" t="n">
         <v>2011</v>
       </c>
     </row>
@@ -982,7 +982,7 @@
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1021,7 +1021,7 @@
       <c r="V4" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W4" s="2" t="n">
+      <c r="W4" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1080,7 +1080,7 @@
       <c r="V5" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W5" s="2" t="n">
+      <c r="W5" s="1" t="n">
         <v>2018</v>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1139,7 +1139,7 @@
       <c r="V6" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W6" s="2" t="n">
+      <c r="W6" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1192,7 +1192,7 @@
       <c r="V7" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W7" s="2" t="n">
+      <c r="W7" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1251,7 +1251,7 @@
       <c r="V8" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W8" s="2" t="n">
+      <c r="W8" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1322,7 +1322,7 @@
       <c r="V9" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W9" s="2" t="n">
+      <c r="W9" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
       <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1381,7 +1381,7 @@
       <c r="V10" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W10" s="2" t="n">
+      <c r="W10" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1440,7 +1440,7 @@
       <c r="V11" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W11" s="2" t="n">
+      <c r="W11" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1454,7 +1454,7 @@
       <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1499,7 +1499,7 @@
       <c r="V12" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W12" s="2" t="n">
+      <c r="W12" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       <c r="C13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1570,7 +1570,7 @@
       <c r="V13" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W13" s="2" t="n">
+      <c r="W13" s="1" t="n">
         <v>1999</v>
       </c>
     </row>
@@ -1584,7 +1584,7 @@
       <c r="C14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1641,7 +1641,7 @@
       <c r="V14" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W14" s="2" t="n">
+      <c r="W14" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1712,7 +1712,7 @@
       <c r="V15" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W15" s="2" t="n">
+      <c r="W15" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1771,7 +1771,7 @@
       <c r="V16" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="W16" s="2" t="n">
+      <c r="W16" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1830,7 +1830,7 @@
       <c r="V17" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W17" s="2" t="n">
+      <c r="W17" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1844,7 +1844,7 @@
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1889,7 +1889,7 @@
       <c r="V18" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W18" s="2" t="n">
+      <c r="W18" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="1" t="n">
         <v>69115</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1948,7 +1948,7 @@
       <c r="V19" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W19" s="2" t="n">
+      <c r="W19" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -1962,7 +1962,7 @@
       <c r="C20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2001,7 +2001,7 @@
       <c r="V20" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W20" s="2" t="n">
+      <c r="W20" s="1" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -2015,7 +2015,7 @@
       <c r="C21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2054,7 +2054,7 @@
       <c r="V21" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W21" s="2" t="n">
+      <c r="W21" s="1" t="n">
         <v>2012</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
       <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2107,7 +2107,7 @@
       <c r="V22" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W22" s="2" t="n">
+      <c r="W22" s="1" t="n">
         <v>2012</v>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2178,7 +2178,7 @@
       <c r="V23" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W23" s="2" t="n">
+      <c r="W23" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -2192,7 +2192,7 @@
       <c r="C24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2249,7 +2249,7 @@
       <c r="V24" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W24" s="2" t="n">
+      <c r="W24" s="1" t="n">
         <v>1999</v>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       <c r="C25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -2308,7 +2308,7 @@
       <c r="V25" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W25" s="2" t="n">
+      <c r="W25" s="1" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -2322,7 +2322,7 @@
       <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2367,7 +2367,7 @@
       <c r="V26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W26" s="2" t="n">
+      <c r="W26" s="1" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       <c r="C27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2426,7 +2426,7 @@
       <c r="V27" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W27" s="2" t="n">
+      <c r="W27" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2479,7 +2479,7 @@
       <c r="V28" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="W28" s="2" t="n">
+      <c r="W28" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2493,7 +2493,7 @@
       <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -2532,7 +2532,7 @@
       <c r="V29" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="W29" s="2" t="n">
+      <c r="W29" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       <c r="C30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -2591,7 +2591,7 @@
       <c r="V30" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W30" s="2" t="n">
+      <c r="W30" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -2605,7 +2605,7 @@
       <c r="C31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="1" t="n">
         <v>69117</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2650,7 +2650,7 @@
       <c r="V31" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W31" s="2" t="n">
+      <c r="W31" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -2664,7 +2664,7 @@
       <c r="C32" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="1" t="n">
         <v>69118</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -2709,7 +2709,7 @@
       <c r="V32" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W32" s="2" t="n">
+      <c r="W32" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
       <c r="C33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="1" t="n">
         <v>69118</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -2768,7 +2768,7 @@
       <c r="V33" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W33" s="2" t="n">
+      <c r="W33" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2782,7 +2782,7 @@
       <c r="C34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="1" t="n">
         <v>69118</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -2827,7 +2827,7 @@
       <c r="V34" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W34" s="2" t="n">
+      <c r="W34" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       <c r="C35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="1" t="n">
         <v>69118</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2898,7 +2898,7 @@
       <c r="V35" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W35" s="2" t="n">
+      <c r="W35" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2912,7 +2912,7 @@
       <c r="C36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="1" t="n">
         <v>69118</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -2957,7 +2957,7 @@
       <c r="V36" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W36" s="2" t="n">
+      <c r="W36" s="1" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
       <c r="C37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -3016,7 +3016,7 @@
       <c r="V37" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W37" s="2" t="n">
+      <c r="W37" s="1" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
       <c r="C38" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -3075,7 +3075,7 @@
       <c r="V38" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W38" s="2" t="n">
+      <c r="W38" s="1" t="n">
         <v>2018</v>
       </c>
     </row>
@@ -3089,7 +3089,7 @@
       <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -3140,7 +3140,7 @@
       <c r="V39" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="W39" s="2" t="n">
+      <c r="W39" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -3154,7 +3154,7 @@
       <c r="C40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -3199,7 +3199,7 @@
       <c r="V40" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W40" s="2" t="n">
+      <c r="W40" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
       <c r="C41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3270,7 +3270,7 @@
       <c r="V41" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W41" s="2" t="n">
+      <c r="W41" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -3284,7 +3284,7 @@
       <c r="C42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3329,7 +3329,7 @@
       <c r="V42" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="W42" s="2" t="n">
+      <c r="W42" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3343,7 +3343,7 @@
       <c r="C43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -3388,7 +3388,7 @@
       <c r="V43" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W43" s="2" t="n">
+      <c r="W43" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3402,7 +3402,7 @@
       <c r="C44" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="1" t="n">
         <v>69120</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -3441,7 +3441,7 @@
       <c r="V44" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="W44" s="2" t="n">
+      <c r="W44" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
@@ -3455,7 +3455,7 @@
       <c r="C45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="1" t="n">
         <v>69121</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3512,7 +3512,7 @@
       <c r="V45" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W45" s="2" t="n">
+      <c r="W45" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       <c r="C46" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="1" t="n">
         <v>69121</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3583,7 +3583,7 @@
       <c r="V46" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W46" s="2" t="n">
+      <c r="W46" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       <c r="C47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="D47" s="1" t="n">
         <v>69121</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3642,7 +3642,7 @@
       <c r="V47" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W47" s="2" t="n">
+      <c r="W47" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       <c r="C48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D48" s="2" t="n">
+      <c r="D48" s="1" t="n">
         <v>69121</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3713,7 +3713,7 @@
       <c r="V48" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W48" s="2" t="n">
+      <c r="W48" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
       <c r="C49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="D49" s="1" t="n">
         <v>69121</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -3772,7 +3772,7 @@
       <c r="V49" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W49" s="2" t="n">
+      <c r="W49" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       <c r="C50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="2" t="n">
+      <c r="D50" s="1" t="n">
         <v>69123</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3831,7 +3831,7 @@
       <c r="V50" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W50" s="2" t="n">
+      <c r="W50" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="C51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="1" t="n">
         <v>69123</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -3902,7 +3902,7 @@
       <c r="V51" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W51" s="2" t="n">
+      <c r="W51" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3916,7 +3916,7 @@
       <c r="C52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="1" t="n">
         <v>69123</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -3967,7 +3967,7 @@
       <c r="V52" s="1" t="n">
         <v>322</v>
       </c>
-      <c r="W52" s="2" t="n">
+      <c r="W52" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       <c r="C53" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D53" s="1" t="n">
         <v>69123</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -4026,7 +4026,7 @@
       <c r="V53" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W53" s="2" t="n">
+      <c r="W53" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4040,7 +4040,7 @@
       <c r="C54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="2" t="n">
+      <c r="D54" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -4085,7 +4085,7 @@
       <c r="V54" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="W54" s="2" t="n">
+      <c r="W54" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
       <c r="C55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="2" t="n">
+      <c r="D55" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -4156,7 +4156,7 @@
       <c r="V55" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W55" s="2" t="n">
+      <c r="W55" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4170,7 +4170,7 @@
       <c r="C56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="2" t="n">
+      <c r="D56" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -4227,7 +4227,7 @@
       <c r="V56" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W56" s="2" t="n">
+      <c r="W56" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4241,7 +4241,7 @@
       <c r="C57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -4286,7 +4286,7 @@
       <c r="V57" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W57" s="2" t="n">
+      <c r="W57" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4300,7 +4300,7 @@
       <c r="C58" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="2" t="n">
+      <c r="D58" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -4357,7 +4357,7 @@
       <c r="V58" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W58" s="2" t="n">
+      <c r="W58" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4371,7 +4371,7 @@
       <c r="C59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="2" t="n">
+      <c r="D59" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -4416,7 +4416,7 @@
       <c r="V59" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W59" s="2" t="n">
+      <c r="W59" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -4430,7 +4430,7 @@
       <c r="C60" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -4487,7 +4487,7 @@
       <c r="V60" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W60" s="2" t="n">
+      <c r="W60" s="1" t="n">
         <v>1999</v>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       <c r="C61" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D61" s="2" t="n">
+      <c r="D61" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -4558,7 +4558,7 @@
       <c r="V61" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="W61" s="2" t="n">
+      <c r="W61" s="1" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -4572,7 +4572,7 @@
       <c r="C62" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D62" s="2" t="n">
+      <c r="D62" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -4617,7 +4617,7 @@
       <c r="V62" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W62" s="2" t="n">
+      <c r="W62" s="1" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -4631,7 +4631,7 @@
       <c r="C63" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>69124</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -4682,7 +4682,7 @@
       <c r="V63" s="1" t="n">
         <v>322</v>
       </c>
-      <c r="W63" s="2" t="n">
+      <c r="W63" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -4696,7 +4696,7 @@
       <c r="C64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -4741,7 +4741,7 @@
       <c r="V64" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W64" s="2" t="n">
+      <c r="W64" s="1" t="n">
         <v>2019</v>
       </c>
     </row>
@@ -4755,7 +4755,7 @@
       <c r="C65" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D65" s="2" t="n">
+      <c r="D65" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -4800,7 +4800,7 @@
       <c r="V65" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W65" s="2" t="n">
+      <c r="W65" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
       <c r="C66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -4859,7 +4859,7 @@
       <c r="V66" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W66" s="2" t="n">
+      <c r="W66" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4873,7 +4873,7 @@
       <c r="C67" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="2" t="n">
+      <c r="D67" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -4918,7 +4918,7 @@
       <c r="V67" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W67" s="2" t="n">
+      <c r="W67" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4932,7 +4932,7 @@
       <c r="C68" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D68" s="2" t="n">
+      <c r="D68" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -4977,7 +4977,7 @@
       <c r="V68" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W68" s="2" t="n">
+      <c r="W68" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -4991,7 +4991,7 @@
       <c r="C69" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D69" s="2" t="n">
+      <c r="D69" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E69" s="1" t="s">
@@ -5030,7 +5030,7 @@
       <c r="V69" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="W69" s="2" t="n">
+      <c r="W69" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
       <c r="C70" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D70" s="2" t="n">
+      <c r="D70" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E70" s="1" t="s">
@@ -5083,7 +5083,7 @@
       <c r="V70" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="W70" s="2" t="n">
+      <c r="W70" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5097,7 +5097,7 @@
       <c r="C71" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D71" s="2" t="n">
+      <c r="D71" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -5148,7 +5148,7 @@
       <c r="V71" s="1" t="n">
         <v>322</v>
       </c>
-      <c r="W71" s="2" t="n">
+      <c r="W71" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
       <c r="C72" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D72" s="2" t="n">
+      <c r="D72" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -5207,7 +5207,7 @@
       <c r="V72" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W72" s="2" t="n">
+      <c r="W72" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5221,7 +5221,7 @@
       <c r="C73" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -5266,7 +5266,7 @@
       <c r="V73" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W73" s="2" t="n">
+      <c r="W73" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5280,7 +5280,7 @@
       <c r="C74" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D74" s="2" t="n">
+      <c r="D74" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E74" s="1" t="s">
@@ -5325,7 +5325,7 @@
       <c r="V74" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W74" s="2" t="n">
+      <c r="W74" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5339,7 +5339,7 @@
       <c r="C75" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D75" s="2" t="n">
+      <c r="D75" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -5384,7 +5384,7 @@
       <c r="V75" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W75" s="2" t="n">
+      <c r="W75" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -5398,7 +5398,7 @@
       <c r="C76" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D76" s="2" t="n">
+      <c r="D76" s="1" t="n">
         <v>69126</v>
       </c>
       <c r="E76" s="1" t="s">
@@ -5443,7 +5443,7 @@
       <c r="V76" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="W76" s="2" t="n">
+      <c r="W76" s="1" t="n">
         <v>2020</v>
       </c>
     </row>

</xml_diff>